<commit_message>
Datos Pruebas y Postman
</commit_message>
<xml_diff>
--- a/Taller2-04-r.cardenas11-f.martinez11/docs/Pruebas.xlsx
+++ b/Taller2-04-r.cardenas11-f.martinez11/docs/Pruebas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -36,10 +36,16 @@
     <t>Se actualiza alguna de las bodegas. En la tabla alojamiento_bodega. Se elimina la fila correspondiente de la tabla Cargar_maritima.</t>
   </si>
   <si>
-    <t>id_carga: 1, id_buque:20</t>
-  </si>
-  <si>
     <t>No se deben actualizar las tablas alojamiento_bodega ni Cargar_maritima, ya que dicho buque no posee la carga descrita.</t>
+  </si>
+  <si>
+    <t>id_carga: 20, id_buque:1</t>
+  </si>
+  <si>
+    <t>id_carga: 2, id_buque:2</t>
+  </si>
+  <si>
+    <t>id_carga: 3, id_buque:3</t>
   </si>
 </sst>
 </file>
@@ -381,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +430,32 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>